<commit_message>
Commit final de  9/7/14
</commit_message>
<xml_diff>
--- a/DB_folder/Config_TetraCam_db.xlsx
+++ b/DB_folder/Config_TetraCam_db.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Estándar" sheetId="1" r:id="rId1"/>
-    <sheet name="Hemav_1" sheetId="2" r:id="rId2"/>
-    <sheet name="Hemav_2" sheetId="3" r:id="rId3"/>
+    <sheet name="Estandar (ilerdair)" sheetId="1" r:id="rId1"/>
+    <sheet name="Vol 1 Algerri" sheetId="2" r:id="rId2"/>
+    <sheet name="Vol 2 Algerri" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
   <si>
     <t>master</t>
   </si>
@@ -37,6 +37,18 @@
   </si>
   <si>
     <t>R730</t>
+  </si>
+  <si>
+    <t>R800</t>
+  </si>
+  <si>
+    <t>R720</t>
+  </si>
+  <si>
+    <t>R530</t>
+  </si>
+  <si>
+    <t>R570</t>
   </si>
 </sst>
 </file>
@@ -381,23 +393,23 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -405,7 +417,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -413,7 +425,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -421,7 +433,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -429,7 +441,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -444,24 +456,126 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Working con proyecto Algerri
</commit_message>
<xml_diff>
--- a/DB_folder/Config_TetraCam_db.xlsx
+++ b/DB_folder/Config_TetraCam_db.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Estandar (ilerdair)" sheetId="1" r:id="rId1"/>
-    <sheet name="Vol 1 Algerri" sheetId="2" r:id="rId2"/>
-    <sheet name="Vol 2 Algerri" sheetId="3" r:id="rId3"/>
+    <sheet name="Config 1 Algerri" sheetId="2" r:id="rId2"/>
+    <sheet name="Config 2 Algerri" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -392,7 +392,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Añadida la configuración de TetraCam para las pruebas RGBN
</commit_message>
<xml_diff>
--- a/DB_folder/Config_TetraCam_db.xlsx
+++ b/DB_folder/Config_TetraCam_db.xlsx
@@ -4,19 +4,20 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Estandar (ilerdair)" sheetId="1" r:id="rId1"/>
-    <sheet name="Config 1 Algerri" sheetId="2" r:id="rId2"/>
-    <sheet name="Config 2 Algerri" sheetId="3" r:id="rId3"/>
+    <sheet name="RGBN Pruebas" sheetId="4" r:id="rId2"/>
+    <sheet name="Config 1 Algerri" sheetId="2" r:id="rId3"/>
+    <sheet name="Config 2 Algerri" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
   <si>
     <t>master</t>
   </si>
@@ -458,8 +459,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,7 +470,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -509,7 +510,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
@@ -521,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,6 +533,69 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Cambios para AB F2 (configuraciones, indices etc)
</commit_message>
<xml_diff>
--- a/DB_folder/Config_TetraCam_db.xlsx
+++ b/DB_folder/Config_TetraCam_db.xlsx
@@ -4,20 +4,22 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Estandar (ilerdair)" sheetId="1" r:id="rId1"/>
     <sheet name="RGBN Pruebas" sheetId="4" r:id="rId2"/>
     <sheet name="Config 1 Algerri" sheetId="2" r:id="rId3"/>
     <sheet name="Config 2 Algerri" sheetId="3" r:id="rId4"/>
+    <sheet name="AB F2 C1" sheetId="5" r:id="rId5"/>
+    <sheet name="AB F2 C2" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="13">
   <si>
     <t>master</t>
   </si>
@@ -50,13 +52,19 @@
   </si>
   <si>
     <t>R570</t>
+  </si>
+  <si>
+    <t>R700</t>
+  </si>
+  <si>
+    <t>R950</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,16 +72,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -81,12 +101,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -397,12 +437,12 @@
       <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>0</v>
       </c>
@@ -410,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -418,7 +458,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -426,7 +466,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -434,7 +474,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -442,7 +482,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -459,13 +499,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,7 +513,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -481,7 +521,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -489,7 +529,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -497,7 +537,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -505,7 +545,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -526,9 +566,9 @@
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,7 +576,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -544,7 +584,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -552,7 +592,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -560,7 +600,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -568,7 +608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -589,9 +629,9 @@
       <selection sqref="A1:B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -599,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -607,7 +647,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -615,7 +655,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -623,7 +663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -631,13 +671,151 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="3"/>
+    </row>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="3"/>
+    </row>
+    <row r="5" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3"/>
+    </row>
+    <row r="6" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>